<commit_message>
Sicherung 03.12. 17:41 Uhr: LCA Funktionen abgeschlossen, Ausgabeübersicht etabliert.
</commit_message>
<xml_diff>
--- a/content/plastiq_input_information.xlsx
+++ b/content/plastiq_input_information.xlsx
@@ -547,7 +547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H22"/>
@@ -683,6 +683,126 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:09:35</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:51:30</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:55:02</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:55:05</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:55:08</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:55:08</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:56:33</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:56:34</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -697,7 +817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G65" sqref="G65"/>
@@ -882,6 +1002,454 @@
         <v>10.00010726291456</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:10:07</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:51:55</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:55:38</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M6" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-03 08:08:41</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:00:51</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:01:58</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:04:08</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M10" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:56:57</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:59:06</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -896,7 +1464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E18"/>
@@ -1038,6 +1606,156 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:10:27</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PVC-P', 'Kupfer']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[20.0, 50.0, 30.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:52:20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['PS', 'PE-HD', 'Chrom']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:56:02</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PEEK', 'Chrom']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[50.0, 30.0, 20.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-03 08:09:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['PP', 'Aluminium', 'PS']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:07:06</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'Aluminium']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:59:39</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'ABS', 'Chrom']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['', '', '']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -1052,7 +1770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F12"/>
@@ -1140,6 +1858,76 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:10:38</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Spritzguss</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:52:29</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Spritzguss</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:07:15</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:59:50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -1154,7 +1942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -1381,6 +2169,153 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:10:57</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>bunt</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[['Gleitmittel'], ['Flammschutzmittel'], ['Biozide']]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:56:19</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>grün</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:07:33</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>braun</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-03 13:01:40</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>bunt</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[['Gleitmittel'], [], []]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>[[], ['Glimmer'], []]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -1395,7 +2330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -1503,6 +2438,66 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:11:40</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[['Gleitmittel'], ['Flammschutzmittel'], ['Biozide']]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[[1.0], [1.0], [1.0]]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-12-03 13:01:48</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[['Gleitmittel'], [], []]</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[[5.0], [5.0], [5.0]]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[[], ['Glimmer'], []]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[[], [1.0], [1.0]]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -1517,7 +2512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
@@ -1668,7 +2663,133 @@
           <t>Woche</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:11:48</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Woche</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:52:56</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Quartal</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-03 07:56:32</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Monat</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-12-03 08:09:15</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Monat</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-12-03 10:07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Quartal</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-12-03 13:02:02</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Woche</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Sicherung vor Lösung der Parameter
</commit_message>
<xml_diff>
--- a/content/plastiq_input_information.xlsx
+++ b/content/plastiq_input_information.xlsx
@@ -547,7 +547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H22"/>
@@ -893,6 +893,71 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:10:50</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:45:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:45:46</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Stefan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Trieß</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Scientist</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>s.triess@skz.de</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>+49</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -907,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G65" sqref="G65"/>
@@ -1837,6 +1902,110 @@
         <v>10.00010726291456</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:11:34</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M19" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:46:07</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M20" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1851,7 +2020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E18"/>
@@ -2268,6 +2437,131 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:11:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'ABS', 'Magnesium']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 5.0, 5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:28:05</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PE-MD', 'ABS', 'Magnesium']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 5.0, 5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:28:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'ABS', 'Magnesium']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 5.0, 5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-09 10:11:50</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PS', 'ABS', 'Magnesium']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[80.0, 10.0, 5.0, 5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:46:32</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['PS', 'PET', 'PA', 'Eisen']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[60.0, 20.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -2282,7 +2576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F12"/>
@@ -2465,6 +2759,36 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:11:59</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:46:37</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -2479,7 +2803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -3002,6 +3326,235 @@
       <c r="I13" t="inlineStr">
         <is>
           <t>[[], [], ['Bariumsulfat']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:12:50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>blau</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>100</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>mittel</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:46:50</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>gelb</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>mittel</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-12-09 17:01:04</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>gelb</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>sehr hoch</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-12-09 17:03:09</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>gelb</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>keine</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-12-09 17:03:34</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>gelb</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>100</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-09 17:04:04</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>gelb</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>mittel</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
@@ -3613,7 +4166,48 @@
           <t>Woche</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:13:02</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Woche</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-09 16:47:02</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Monat</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
- Übertragung der Parameter in ein Excel Sheet
</commit_message>
<xml_diff>
--- a/content/plastiq_input_information.xlsx
+++ b/content/plastiq_input_information.xlsx
@@ -547,7 +547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H22"/>
@@ -958,6 +958,36 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:17:54</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:38:23</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -972,7 +1002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G65" sqref="G65"/>
@@ -2006,6 +2036,110 @@
         <v>10.00010726291456</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:18:15</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M21" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:38:44</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>SKZ</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Friedrich-Bergius-Ring 22</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>97076</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Würzburg</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Bayern</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>49.80282025</v>
+      </c>
+      <c r="M22" t="n">
+        <v>10.00010726291456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2020,7 +2154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E18"/>
@@ -2562,6 +2696,106 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:18:43</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'PVC-U', 'SAN']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[50.0, 30.0, 15.0, 5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:39:03</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'PVC-U', 'POM']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[50.0, 30.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:40:30</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['PE-LD', 'PP', 'PVC-U', 'Aluminium']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['', '', '', '']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[50.0, 30.0, 10.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:50:28</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['PP', 'PS']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['', '']</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[50.0, 50.0]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -2576,7 +2810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F12"/>
@@ -2789,6 +3023,21 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:18:47</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -2803,7 +3052,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -3546,7 +3795,6 @@
           <t>mittel</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>[[], [], [], []]</t>
@@ -3555,6 +3803,115 @@
       <c r="I19" t="inlineStr">
         <is>
           <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:19:00</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>braun</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>100</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>mittel</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>[[], [], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:39:15</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>grün</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:50:40</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>gering</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3784,7 +4141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
@@ -4209,6 +4566,70 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:19:10</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Quartal</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:39:24</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Jahr</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-12-09 19:50:49</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Woche</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>